<commit_message>
chore(schema): fix date and some linkml-lint warnings
</commit_message>
<xml_diff>
--- a/project/excel/datatype.xlsx
+++ b/project/excel/datatype.xlsx
@@ -11,10 +11,10 @@
     <sheet name="Boolean" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Concept" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Count" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Quantitative Measure" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Quantitative Range" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="QuantitativeMeasure" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="QuantitativeRange" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Percent" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Percent Range" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="PercentRange" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>